<commit_message>
Added results comparison between liściu and lucas implementations
</commit_message>
<xml_diff>
--- a/henrar/results/results.xlsx
+++ b/henrar/results/results.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DRIVE\GIT\TPRLab5\henrar\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Podstawowy" sheetId="1" r:id="rId1"/>
     <sheet name="Skalowalny" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -38,11 +43,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
+    <numFmt numFmtId="165" formatCode="[$-415]General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +72,12 @@
       <name val="Liberation Sans"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -84,7 +96,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment horizontal="center"/>
@@ -94,11 +106,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Excel Built-in Normal" xfId="5"/>
     <cellStyle name="Heading" xfId="1"/>
     <cellStyle name="Heading1" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -120,7 +135,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -139,14 +164,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -218,10 +249,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -293,10 +328,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -368,16 +407,229 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="97949184"/>
-        <c:axId val="97934720"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2191907695568631</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6718777104713531</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9069935646594089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9135899244859029</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2992224281945841</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5686342453908644</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$M$10:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8991126891953458</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4547241245944944</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3855488887293159</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8750427851391835</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7480792455739138</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6215422319827946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$M$18:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9371595597899653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6912242403400111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1772625751045966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5845900801280264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4580969538813822</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.779238791241033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155341808"/>
+        <c:axId val="-1155342352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97934720"/>
+        <c:axId val="-1155342352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -405,9 +657,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -423,18 +677,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97949184"/>
+        <c:crossAx val="-1155341808"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97949184"/>
+        <c:axId val="-1155341808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -453,9 +708,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -471,10 +728,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97934720"/>
+        <c:crossAx val="-1155342352"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -491,6 +748,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -504,12 +762,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -526,7 +785,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -545,14 +814,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -624,10 +899,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -699,10 +978,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -774,16 +1057,229 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="72108288"/>
-        <c:axId val="72106368"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$N$2:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60959538477843156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91796942761783829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81783226077656812</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86419874056073787</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7544747661995076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71405285378257199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$N$10:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94955634459767291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8636810311486236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73092481478821936</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73438034814239794</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61346174959762856</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.55179518599856625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$N$18:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96857977989498267</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92280606008500277</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86287709585076611</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8230737600160033</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76891790489830747</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73160323260341942</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155332016"/>
+        <c:axId val="-1155338000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72106368"/>
+        <c:axId val="-1155338000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -811,9 +1307,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -829,18 +1327,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72108288"/>
+        <c:crossAx val="-1155332016"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72108288"/>
+        <c:axId val="-1155332016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -859,9 +1358,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -877,10 +1378,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72106368"/>
+        <c:crossAx val="-1155338000"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -897,6 +1398,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -910,12 +1412,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -932,7 +1435,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -951,14 +1464,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1027,10 +1546,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1099,10 +1622,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1171,16 +1698,220 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="72150016"/>
-        <c:axId val="72148096"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$O$2:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>0.64043236705846796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9786965997707176E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.454892475150235E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2448748198020674E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2542537510865867E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6405141402306856E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$O$10:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>5.312339356091611E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2611617767454266E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3625954343811265E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1670315861622518E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3009348285513023E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.3842420549958196E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Podstawowy!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Podstawowy!$O$18:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>3.2439475567437537E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7883771485667157E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1782719650018221E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0708277153774808E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0052895586070938E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3351009180393049E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155344528"/>
+        <c:axId val="-1155336368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72148096"/>
+        <c:axId val="-1155336368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1208,9 +1939,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1226,18 +1959,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72150016"/>
+        <c:crossAx val="-1155344528"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72150016"/>
+        <c:axId val="-1155344528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1256,9 +1990,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1274,10 +2010,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72148096"/>
+        <c:crossAx val="-1155336368"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1294,6 +2030,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1307,12 +2044,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -1329,7 +2067,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1348,14 +2096,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1427,10 +2181,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1502,10 +2260,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1577,16 +2339,229 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="100180352"/>
-        <c:axId val="100174080"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.679090018344028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9032938126765453</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4832537347648338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7607056875841192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0078220441022676</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2949615284583542</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$M$10:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8471358659296551</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3634994005680179</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6110077605678779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8527339762718853</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6752762269259538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0031627708313202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$M$18:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8648598419343354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4981948391900115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7658163142091237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0738943421197744</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.890939810338597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2933818817360909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155335824"/>
+        <c:axId val="-1155337456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100174080"/>
+        <c:axId val="-1155337456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1614,9 +2589,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1632,18 +2609,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100180352"/>
+        <c:crossAx val="-1155335824"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100180352"/>
+        <c:axId val="-1155335824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1662,9 +2640,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1680,10 +2660,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100174080"/>
+        <c:crossAx val="-1155337456"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1700,6 +2680,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1713,12 +2694,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -1735,7 +2717,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1754,14 +2746,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1833,10 +2831,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1908,10 +2910,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -1983,16 +2989,229 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="100508800"/>
-        <c:axId val="100502528"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$N$2:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83954500917201402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72582345316913632</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5805422891274723</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7200882109480149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45525654946384253</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52458012737152948</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$N$10:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92356793296482753</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84087485014200447</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76850129342797968</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73159174703398566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6068432933569049</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66693023090261006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$N$18:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9324299209671677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.87454870979750288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79430271903485394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7592367927649718</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26281271003078155</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10778182347800758</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155338544"/>
+        <c:axId val="-1155339632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100502528"/>
+        <c:axId val="-1155339632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2020,9 +3239,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2038,18 +3259,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100508800"/>
+        <c:crossAx val="-1155338544"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100508800"/>
+        <c:axId val="-1155338544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2068,9 +3290,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2086,10 +3310,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100502528"/>
+        <c:crossAx val="-1155339632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2106,6 +3330,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2119,12 +3344,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2141,7 +3367,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2160,14 +3396,20 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Lucas:1000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -2236,10 +3478,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Lucas:10000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -2308,10 +3554,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Lucas:100000000</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28800">
               <a:solidFill>
@@ -2380,16 +3630,220 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="105224064"/>
-        <c:axId val="105222144"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Liściu:1000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$O$2:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>0.19112136821137415</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12591516832077035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14450548004106742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5531249960825528E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11965636764099366</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2389679222750742E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Liściu:10000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$10:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$O$10:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>[$-415]General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>8.2757385035891362E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3079204486106752E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0246796863384938E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2411794273864061E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.4787188215964436E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5400655893144112E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Liściu:100000000</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Skalowalny!$I$18:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Skalowalny!$O$18:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>7.2466656757158576E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.781562909611773E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.179317054714002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5301734871752312E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28049910138778167</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75254565846839128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1155333104"/>
+        <c:axId val="-1155334192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105222144"/>
+        <c:axId val="-1155334192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2417,9 +3871,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2435,18 +3891,19 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105224064"/>
+        <c:crossAx val="-1155333104"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105224064"/>
+        <c:axId val="-1155333104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2465,9 +3922,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2483,10 +3942,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105222144"/>
+        <c:crossAx val="-1155334192"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2503,6 +3962,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2516,12 +3976,13 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pl-PL"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2540,12 +4001,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142709</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5397840" cy="3237840"/>
+    <xdr:ext cx="5762791" cy="3619500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2565,12 +4026,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>39720</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5400720" cy="3240720"/>
+    <xdr:ext cx="5808630" cy="3648075"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
@@ -2591,9 +4052,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:colOff>230220</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>40980</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400720" cy="3237120"/>
     <xdr:graphicFrame macro="">
@@ -2620,10 +4081,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>325470</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>155640</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400720" cy="3237120"/>
     <xdr:graphicFrame macro="">
@@ -2645,10 +4106,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>173070</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400720" cy="3240720"/>
     <xdr:graphicFrame macro="">
@@ -2670,10 +4131,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>249270</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>136230</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5400720" cy="3237120"/>
     <xdr:graphicFrame macro="">
@@ -2951,28 +4412,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="H22" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="9" width="10.625" customWidth="1"/>
+    <col min="4" max="10" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2992,7 +4453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3010,8 +4471,27 @@
         <f t="shared" ref="F2:F8" si="0">E2/A2</f>
         <v>1</v>
       </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.26458999999999999</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1">
+        <f>K2/K2</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" ref="N2:N8" si="1">M2/I2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3030,11 +4510,33 @@
         <v>0.75617560159556052</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="1">(1/E3-1/A3)/(1-1/A3)</f>
+        <f t="shared" ref="G3:G8" si="2">(1/E3-1/A3)/(1-1/A3)</f>
         <v>0.32244414907061314</v>
       </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.21702099999999999</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <f>K2/K3</f>
+        <v>1.2191907695568631</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="1"/>
+        <v>0.60959538477843156</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O8" si="3">(1/M3-1/I3)/(1-1/I3)</f>
+        <v>0.64043236705846796</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3053,11 +4555,33 @@
         <v>0.67927809646925752</v>
       </c>
       <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.15738370150987566</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>7.2058499999999998E-2</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <f>K2/K4</f>
+        <v>3.6718777104713531</v>
+      </c>
+      <c r="N4" s="1">
         <f t="shared" si="1"/>
-        <v>0.15738370150987566</v>
+        <v>0.91796942761783829</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="3"/>
+        <v>2.9786965997707176E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3076,11 +4600,33 @@
         <v>0.6772535041082649</v>
       </c>
       <c r="G5">
+        <f t="shared" si="2"/>
+        <v>9.5310395275604573E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.3920999999999997E-2</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <f>K2/K5</f>
+        <v>4.9069935646594089</v>
+      </c>
+      <c r="N5" s="1">
         <f t="shared" si="1"/>
-        <v>9.5310395275604573E-2</v>
+        <v>0.81783226077656812</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="3"/>
+        <v>4.454892475150235E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3099,11 +4645,33 @@
         <v>0.62007146650146039</v>
       </c>
       <c r="G6">
+        <f t="shared" si="2"/>
+        <v>8.7531047173862869E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3.8270999999999999E-2</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <f>K2/K6</f>
+        <v>6.9135899244859029</v>
+      </c>
+      <c r="N6" s="1">
         <f t="shared" si="1"/>
-        <v>8.7531047173862869E-2</v>
+        <v>0.86419874056073787</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2448748198020674E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3122,11 +4690,33 @@
         <v>0.61077168958064698</v>
       </c>
       <c r="G7">
+        <f t="shared" si="2"/>
+        <v>7.0808111745140595E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3.1881300000000001E-2</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <f>K2/K7</f>
+        <v>8.2992224281945841</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="1"/>
-        <v>7.0808111745140595E-2</v>
+        <v>0.7544747661995076</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="3"/>
+        <v>3.2542537510865867E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3145,11 +4735,42 @@
         <v>0.60869116656892774</v>
       </c>
       <c r="G8">
+        <f t="shared" si="2"/>
+        <v>5.844265904569744E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>12</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3.0878900000000001E-2</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1">
+        <f>K2/K8</f>
+        <v>8.5686342453908644</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="1"/>
-        <v>5.844265904569744E-2</v>
+        <v>0.71405285378257199</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6405141402306856E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="9" spans="1:15">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3164,11 +4785,30 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="2">E10/A10</f>
+        <f t="shared" ref="F10:F16" si="4">E10/A10</f>
         <v>1</v>
       </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2.62615</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <f>K10/K10</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" ref="N10:N16" si="5">M10/I10</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3183,15 +4823,37 @@
         <v>1.8637518550570085</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.93187592752850423</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G16" si="3">(1/E11-1/A11)/(1-1/A11)</f>
+        <f t="shared" ref="G11:G16" si="6">(1/E11-1/A11)/(1-1/A11)</f>
         <v>7.3104230358404632E-2</v>
       </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.38283</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1">
+        <f>K10/K11</f>
+        <v>1.8991126891953458</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.94955634459767291</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O16" si="7">(1/M11-1/I11)/(1-1/I11)</f>
+        <v>5.312339356091611E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3206,15 +4868,37 @@
         <v>3.4255924925502894</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.85639812313757235</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.5893737963956802E-2</v>
       </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.760162</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1">
+        <f>K10/K12</f>
+        <v>3.4547241245944944</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.8636810311486236</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="7"/>
+        <v>5.2611617767454266E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3229,15 +4913,37 @@
         <v>4.5468063177738038</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.7578010529623006</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.392151240511626E-2</v>
       </c>
+      <c r="I13" s="1">
+        <v>6</v>
+      </c>
+      <c r="J13" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.59881899999999999</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1">
+        <f>K10/K13</f>
+        <v>4.3855488887293159</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.73092481478821936</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="7"/>
+        <v>7.3625954343811265E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>8</v>
       </c>
@@ -3252,15 +4958,37 @@
         <v>5.2441224879604986</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.65551531099506233</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.5073911476718366E-2</v>
       </c>
+      <c r="I14" s="1">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.44700099999999998</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1">
+        <f>K10/K14</f>
+        <v>5.8750427851391835</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.73438034814239794</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1670315861622518E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>10</v>
       </c>
@@ -3275,15 +5003,37 @@
         <v>6.2232073064132054</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.62232073064132054</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.7432051024284415E-2</v>
       </c>
+      <c r="I15" s="1">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.38917000000000002</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1">
+        <f>K10/K15</f>
+        <v>6.7480792455739138</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.61346174959762856</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="7"/>
+        <v>6.3009348285513023E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3298,15 +5048,46 @@
         <v>7.0288535082443451</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.58573779235369539</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4295323243164823E-2</v>
       </c>
+      <c r="I16" s="1">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.39660699999999999</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
+        <f>K10/K16</f>
+        <v>6.6215422319827946</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="5"/>
+        <v>0.55179518599856625</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="7"/>
+        <v>7.3842420549958196E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="17" spans="1:15">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3321,11 +5102,30 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18:F24" si="4">E18/A18</f>
+        <f t="shared" ref="F18:F24" si="8">E18/A18</f>
         <v>1</v>
       </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>29.624400000000001</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1">
+        <f>K18/K18</f>
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" ref="N18:N24" si="9">M18/I18</f>
+        <v>1</v>
+      </c>
+      <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3340,15 +5140,37 @@
         <v>1.8931801806536117</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.94659009032680586</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G24" si="5">(1/E19-1/A19)/(1-1/A19)</f>
+        <f t="shared" ref="G19:G24" si="10">(1/E19-1/A19)/(1-1/A19)</f>
         <v>5.6423482792593571E-2</v>
       </c>
+      <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>15.2927</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1">
+        <f>K18/K19</f>
+        <v>1.9371595597899653</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="9"/>
+        <v>0.96857977989498267</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" ref="O19:O24" si="11">(1/M19-1/I19)/(1-1/I19)</f>
+        <v>3.2439475567437537E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3363,15 +5185,37 @@
         <v>3.6482048027732072</v>
       </c>
       <c r="F20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.91205120069330181</v>
       </c>
       <c r="G20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.2143224430033181E-2</v>
       </c>
+      <c r="I20" s="1">
+        <v>4</v>
+      </c>
+      <c r="J20" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>8.0256299999999996</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1">
+        <f>K18/K20</f>
+        <v>3.6912242403400111</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="9"/>
+        <v>0.92280606008500277</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="11"/>
+        <v>2.7883771485667157E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>6</v>
       </c>
@@ -3386,15 +5230,37 @@
         <v>5.0608872892978161</v>
       </c>
       <c r="F21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.84348121488296934</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.7112571650750326E-2</v>
       </c>
+      <c r="I21" s="1">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5.7220199999999997</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1">
+        <f>K18/K21</f>
+        <v>5.1772625751045966</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="9"/>
+        <v>0.86287709585076611</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="11"/>
+        <v>3.1782719650018221E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>8</v>
       </c>
@@ -3409,15 +5275,37 @@
         <v>6.2316829248635957</v>
       </c>
       <c r="F22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.77896036560794946</v>
       </c>
       <c r="G22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.0537480495289442E-2</v>
       </c>
+      <c r="I22" s="1">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K22" s="1">
+        <v>4.4990500000000004</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1">
+        <f>K18/K22</f>
+        <v>6.5845900801280264</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="9"/>
+        <v>0.8230737600160033</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="11"/>
+        <v>3.0708277153774808E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>10</v>
       </c>
@@ -3432,15 +5320,37 @@
         <v>7.0462050032318606</v>
       </c>
       <c r="F23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.70462050032318602</v>
       </c>
       <c r="G23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.6578185553048011E-2</v>
       </c>
+      <c r="I23" s="1">
+        <v>11</v>
+      </c>
+      <c r="J23" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>3.5024899999999999</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1">
+        <f>K18/K23</f>
+        <v>8.4580969538813822</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="9"/>
+        <v>0.76891790489830747</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="11"/>
+        <v>3.0052895586070938E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>12</v>
       </c>
@@ -3455,12 +5365,34 @@
         <v>8.0083726351996063</v>
       </c>
       <c r="F24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.66736438626663386</v>
       </c>
       <c r="G24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.5311979288637276E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>12</v>
+      </c>
+      <c r="J24" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K24" s="1">
+        <v>3.3743699999999999</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1">
+        <f>K18/K24</f>
+        <v>8.779238791241033</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="9"/>
+        <v>0.73160323260341942</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="11"/>
+        <v>3.3351009180393049E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3474,11 +5406,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3487,9 +5419,10 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="8" width="10.625" customWidth="1"/>
+    <col min="10" max="10" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3509,7 +5442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3528,13 +5461,32 @@
         <f t="shared" ref="F2:F8" si="0">E2/A2</f>
         <v>1</v>
       </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.22791800000000001</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1">
+        <f>K2/K2</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" ref="N2:N8" si="1">M2/I2</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B8" si="1">1000000*A3</f>
+        <f t="shared" ref="B3:B8" si="2">1000000*A3</f>
         <v>2000000</v>
       </c>
       <c r="C3">
@@ -3550,16 +5502,39 @@
         <v>0.89786544608545393</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="2">(1/E3-1/A3)/(1-1/A3)</f>
+        <f t="shared" ref="G3:G8" si="3">(1/E3-1/A3)/(1-1/A3)</f>
         <v>0.11375262781281537</v>
       </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K3" s="1">
+        <f>0.271478/2</f>
+        <v>0.135739</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <f>K2/K3</f>
+        <v>1.679090018344028</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83954500917201402</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O8" si="4">(1/M3-1/I3)/(1-1/I3)</f>
+        <v>0.19112136821137415</v>
+      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000000</v>
       </c>
       <c r="C4">
@@ -3575,16 +5550,39 @@
         <v>0.75176416342568464</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11006813424178989</v>
       </c>
+      <c r="I4" s="1">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K4" s="1">
+        <f>0.314013/4</f>
+        <v>7.8503249999999997E-2</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <f>K2/K4</f>
+        <v>2.9032938126765453</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.72582345316913632</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="4"/>
+        <v>0.12591516832077035</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6000000</v>
       </c>
       <c r="C5">
@@ -3600,16 +5598,39 @@
         <v>0.58975696446732451</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13912274385880699</v>
       </c>
+      <c r="I5" s="1">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K5" s="1">
+        <f>0.392595/6</f>
+        <v>6.5432500000000005E-2</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <f>K2/K5</f>
+        <v>3.4832537347648338</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5805422891274723</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="4"/>
+        <v>0.14450548004106742</v>
+      </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8000000</v>
       </c>
       <c r="C6">
@@ -3625,16 +5646,39 @@
         <v>0.5403022851489333</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12154511266499426</v>
       </c>
+      <c r="I6" s="1">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K6" s="1">
+        <f>0.316514/8</f>
+        <v>3.9564250000000002E-2</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <f>K2/K6</f>
+        <v>5.7607056875841192</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7200882109480149</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="4"/>
+        <v>5.5531249960825528E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="C7">
@@ -3650,16 +5694,39 @@
         <v>0.46775464382607607</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12643032771301152</v>
       </c>
+      <c r="I7" s="1">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="1">
+        <f>0.455124/10</f>
+        <v>4.5512399999999995E-2</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <f>K2/K7</f>
+        <v>5.0078220441022676</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45525654946384253</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11965636764099366</v>
+      </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12000000</v>
       </c>
       <c r="C8">
@@ -3675,11 +5742,43 @@
         <v>0.4987685793773069</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.1357985783244777E-2</v>
       </c>
+      <c r="I8" s="1">
+        <v>12</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K8" s="1">
+        <f>0.434477/12</f>
+        <v>3.6206416666666665E-2</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1">
+        <f>K2/K8</f>
+        <v>6.2949615284583542</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.52458012737152948</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="4"/>
+        <v>8.2389679222750742E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="9" spans="1:15">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3695,16 +5794,35 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F16" si="3">E10/A10</f>
+        <f t="shared" ref="F10:F16" si="5">E10/A10</f>
         <v>1</v>
       </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2.6232099999999998</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <f>K10/K10</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" ref="N10:N16" si="6">M10/I10</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B16" si="4">1000000*A11</f>
+        <f t="shared" ref="B11:B16" si="7">1000000*A11</f>
         <v>2000000</v>
       </c>
       <c r="C11">
@@ -3716,20 +5834,43 @@
         <v>1.7909384071862846</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.8954692035931423</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G16" si="5">(1/E11-1/A11)/(1-1/A11)</f>
+        <f t="shared" ref="G11:G16" si="8">(1/E11-1/A11)/(1-1/A11)</f>
         <v>0.11673298868059279</v>
       </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K11" s="1">
+        <f>2.8403/2</f>
+        <v>1.42015</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1">
+        <f>K10/K11</f>
+        <v>1.8471358659296551</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.92356793296482753</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O16" si="9">(1/M11-1/I11)/(1-1/I11)</f>
+        <v>8.2757385035891362E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4000000</v>
       </c>
       <c r="C12">
@@ -3741,20 +5882,43 @@
         <v>3.1657567553502424</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.79143918883756059</v>
       </c>
       <c r="G12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.7840318457807001E-2</v>
       </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K12" s="1">
+        <f>3.11962/4</f>
+        <v>0.77990499999999996</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1">
+        <f>K10/K12</f>
+        <v>3.3634994005680179</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="6"/>
+        <v>0.84087485014200447</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="9"/>
+        <v>6.3079204486106752E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6000000</v>
       </c>
       <c r="C13">
@@ -3766,20 +5930,43 @@
         <v>4.2219758711001978</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.7036626451833663</v>
       </c>
       <c r="G13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.4227109921235541E-2</v>
       </c>
+      <c r="I13" s="1">
+        <v>6</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="1">
+        <f>3.41341/6</f>
+        <v>0.56890166666666664</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1">
+        <f>K10/K13</f>
+        <v>4.6110077605678779</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="6"/>
+        <v>0.76850129342797968</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="9"/>
+        <v>6.0246796863384938E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8000000</v>
       </c>
       <c r="C14">
@@ -3791,20 +5978,43 @@
         <v>4.9467937134714433</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.61834921418393041</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>8.8172734080081555E-2</v>
       </c>
+      <c r="I14" s="1">
+        <v>8</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K14" s="1">
+        <f>3.58562/8</f>
+        <v>0.4482025</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1">
+        <f>K10/K14</f>
+        <v>5.8527339762718853</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.73159174703398566</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="9"/>
+        <v>5.2411794273864061E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>10</v>
       </c>
       <c r="B15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>10000000</v>
       </c>
       <c r="C15">
@@ -3816,20 +6026,43 @@
         <v>6.153758023399484</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.61537580233994837</v>
       </c>
       <c r="G15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.9447030253262279E-2</v>
       </c>
+      <c r="I15" s="1">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K15" s="1">
+        <f>3.92974/10</f>
+        <v>0.39297399999999999</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1">
+        <f>K10/K15</f>
+        <v>6.6752762269259538</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="6"/>
+        <v>0.6068432933569049</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="9"/>
+        <v>6.4787188215964436E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12000000</v>
       </c>
       <c r="C16">
@@ -3841,15 +6074,47 @@
         <v>6.5552360816535202</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.54626967347112665</v>
       </c>
       <c r="G16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>7.5508880514131335E-2</v>
       </c>
+      <c r="I16" s="1">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="K16" s="1">
+        <f>3.93326/12</f>
+        <v>0.32777166666666668</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
+        <f>K10/K16</f>
+        <v>8.0031627708313202</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="6"/>
+        <v>0.66693023090261006</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="9"/>
+        <v>4.5400655893144112E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="17" spans="1:15">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3865,16 +6130,35 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18:F24" si="6">E18/A18</f>
+        <f t="shared" ref="F18:F24" si="10">E18/A18</f>
         <v>1</v>
       </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>29.601199999999999</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1">
+        <f>K18/K18</f>
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" ref="N18:N24" si="11">M18/I18</f>
+        <v>1</v>
+      </c>
+      <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B24" si="7">100000000*A19</f>
+        <f t="shared" ref="B19:B24" si="12">100000000*A19</f>
         <v>200000000</v>
       </c>
       <c r="C19">
@@ -3886,20 +6170,43 @@
         <v>1.8221011062972838</v>
       </c>
       <c r="F19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.91105055314864192</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G24" si="8">(1/E19-1/A19)/(1-1/A19)</f>
+        <f t="shared" ref="G19:G24" si="13">(1/E19-1/A19)/(1-1/A19)</f>
         <v>9.7633931008486607E-2</v>
       </c>
+      <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K19" s="1">
+        <f>31.7463/2</f>
+        <v>15.873150000000001</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1">
+        <f>K18/K19</f>
+        <v>1.8648598419343354</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="11"/>
+        <v>0.9324299209671677</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" ref="O19:O24" si="14">(1/M19-1/I19)/(1-1/I19)</f>
+        <v>7.2466656757158576E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>400000000</v>
       </c>
       <c r="C20">
@@ -3911,20 +6218,43 @@
         <v>3.19140663536687</v>
       </c>
       <c r="F20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.79785165884171749</v>
       </c>
       <c r="G20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>8.4455273908833187E-2</v>
       </c>
+      <c r="I20" s="1">
+        <v>4</v>
+      </c>
+      <c r="J20" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K20" s="1">
+        <f>33.8474/4</f>
+        <v>8.4618500000000001</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1">
+        <f>K18/K20</f>
+        <v>3.4981948391900115</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="11"/>
+        <v>0.87454870979750288</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="14"/>
+        <v>4.781562909611773E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>6</v>
       </c>
       <c r="B21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>600000000</v>
       </c>
       <c r="C21">
@@ -3936,20 +6266,43 @@
         <v>4.0311134471339285</v>
       </c>
       <c r="F21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.67185224118898812</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>9.7684502244208743E-2</v>
       </c>
+      <c r="I21" s="1">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K21" s="1">
+        <f>37.2669/6</f>
+        <v>6.2111499999999999</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1">
+        <f>K18/K21</f>
+        <v>4.7658163142091237</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="11"/>
+        <v>0.79430271903485394</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="14"/>
+        <v>5.179317054714002E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>8</v>
       </c>
       <c r="B22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>800000000</v>
       </c>
       <c r="C22">
@@ -3961,20 +6314,43 @@
         <v>5.0787161413672806</v>
       </c>
       <c r="F22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.63483951767091007</v>
       </c>
       <c r="G22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>8.2171606741267542E-2</v>
       </c>
+      <c r="I22" s="1">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K22" s="1">
+        <f>38.9881/8</f>
+        <v>4.8735125000000004</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1">
+        <f>K18/K22</f>
+        <v>6.0738943421197744</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="11"/>
+        <v>0.7592367927649718</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="14"/>
+        <v>4.5301734871752312E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>10</v>
       </c>
       <c r="B23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1000000000</v>
       </c>
       <c r="C23">
@@ -3986,20 +6362,43 @@
         <v>5.7723336838101424</v>
       </c>
       <c r="F23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.57723336838101424</v>
       </c>
       <c r="G23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>8.1377953446518589E-2</v>
       </c>
+      <c r="I23" s="1">
+        <v>11</v>
+      </c>
+      <c r="J23" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K23" s="1">
+        <f>102.393/10</f>
+        <v>10.2393</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1">
+        <f>K18/K23</f>
+        <v>2.890939810338597</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="11"/>
+        <v>0.26281271003078155</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="14"/>
+        <v>0.28049910138778167</v>
+      </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>12</v>
       </c>
       <c r="B24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1200000000</v>
       </c>
       <c r="C24">
@@ -4011,12 +6410,35 @@
         <v>6.7233699907731932</v>
       </c>
       <c r="F24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.56028083256443273</v>
       </c>
       <c r="G24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>7.1347202052057815E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>12</v>
+      </c>
+      <c r="J24" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="K24" s="1">
+        <f>274.64/12</f>
+        <v>22.886666666666667</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1">
+        <f>K18/K24</f>
+        <v>1.2933818817360909</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="11"/>
+        <v>0.10778182347800758</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="14"/>
+        <v>0.75254565846839128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>